<commit_message>
Bunch of UI Updates
1. User View
2. Download User tweets
3. Download All candidate names
4. Added numbers to list (tweets)
</commit_message>
<xml_diff>
--- a/Data/Downloads/all_candidate_names.xlsx
+++ b/Data/Downloads/all_candidate_names.xlsx
@@ -6,7 +6,11 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="binay" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="duterte" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="poe" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="roxas" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="santiago" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,15 +18,510 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="170">
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>jejomar</t>
+  </si>
+  <si>
+    <t>binay</t>
+  </si>
+  <si>
+    <t>binayaran</t>
+  </si>
+  <si>
+    <t>ionnebinay</t>
+  </si>
+  <si>
+    <t>binayarang</t>
+  </si>
+  <si>
+    <t>binayad</t>
+  </si>
+  <si>
+    <t>rodrigo</t>
+  </si>
+  <si>
+    <t>digong</t>
+  </si>
+  <si>
+    <t>du30</t>
+  </si>
+  <si>
+    <t>duterte</t>
+  </si>
+  <si>
+    <t>🙏duterte</t>
+  </si>
+  <si>
+    <t>dudutertehin</t>
+  </si>
+  <si>
+    <t>duterteing</t>
+  </si>
+  <si>
+    <t>pdu30</t>
+  </si>
+  <si>
+    <t>duterte😂</t>
+  </si>
+  <si>
+    <t>du30ng</t>
+  </si>
+  <si>
+    <t>dutertem</t>
+  </si>
+  <si>
+    <t>bbmdu30for</t>
+  </si>
+  <si>
+    <t>naduterte</t>
+  </si>
+  <si>
+    <t>👊✊👮👏🔫🚬🍻👡🚓❌du30</t>
+  </si>
+  <si>
+    <t>duterteon1</t>
+  </si>
+  <si>
+    <t>dutertestop</t>
+  </si>
+  <si>
+    <t>rodydu30</t>
+  </si>
+  <si>
+    <t>duterte~</t>
+  </si>
+  <si>
+    <t>digong😂</t>
+  </si>
+  <si>
+    <t>duterteadministration</t>
+  </si>
+  <si>
+    <t>~duterte</t>
+  </si>
+  <si>
+    <t>dutertex</t>
+  </si>
+  <si>
+    <t>du30✊👊</t>
+  </si>
+  <si>
+    <t>duterte😌😌</t>
+  </si>
+  <si>
+    <t>tataydigong</t>
+  </si>
+  <si>
+    <t>dutertenews</t>
+  </si>
+  <si>
+    <t>makadu30</t>
+  </si>
+  <si>
+    <t>nagduterte</t>
+  </si>
+  <si>
+    <t>rodrigoduterte</t>
+  </si>
+  <si>
+    <t>dutertes</t>
+  </si>
+  <si>
+    <t>grace</t>
+  </si>
+  <si>
+    <t>poe</t>
+  </si>
+  <si>
+    <t>poewszxc</t>
+  </si>
+  <si>
+    <t>disgrace</t>
+  </si>
+  <si>
+    <t>poetic</t>
+  </si>
+  <si>
+    <t>graces</t>
+  </si>
+  <si>
+    <t>sengracepoe</t>
+  </si>
+  <si>
+    <t>poewhsz</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>roxas</t>
+  </si>
+  <si>
+    <t>primarily</t>
+  </si>
+  <si>
+    <t>maris</t>
+  </si>
+  <si>
+    <t>mars</t>
+  </si>
+  <si>
+    <t>nightmarishly</t>
+  </si>
+  <si>
+    <t>martin</t>
+  </si>
+  <si>
+    <t>pinakamaraming</t>
+  </si>
+  <si>
+    <t>marry</t>
+  </si>
+  <si>
+    <t>martínez</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>susmaryosep</t>
+  </si>
+  <si>
+    <t>marehab</t>
+  </si>
+  <si>
+    <t>grammar</t>
+  </si>
+  <si>
+    <t>marlyn</t>
+  </si>
+  <si>
+    <t>alimario</t>
+  </si>
+  <si>
+    <t>marcoses</t>
+  </si>
+  <si>
+    <t>maroxas</t>
+  </si>
+  <si>
+    <t>maranao</t>
+  </si>
+  <si>
+    <t>maranasan</t>
+  </si>
+  <si>
+    <t>umarte</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>humarap</t>
+  </si>
+  <si>
+    <t>marie</t>
+  </si>
+  <si>
+    <t>marlon</t>
+  </si>
+  <si>
+    <t>nightmare</t>
+  </si>
+  <si>
+    <t>marcosparin</t>
+  </si>
+  <si>
+    <t>marlwan</t>
+  </si>
+  <si>
+    <t>marasigan</t>
+  </si>
+  <si>
+    <t>marquez</t>
+  </si>
+  <si>
+    <t>marching</t>
+  </si>
+  <si>
+    <t>martyr</t>
+  </si>
+  <si>
+    <t>marcelino</t>
+  </si>
+  <si>
+    <t>maribojoc</t>
+  </si>
+  <si>
+    <t>martial</t>
+  </si>
+  <si>
+    <t>thisiskorinasanchezroxas</t>
+  </si>
+  <si>
+    <t>smartest</t>
+  </si>
+  <si>
+    <t>mary</t>
+  </si>
+  <si>
+    <t>marinig</t>
+  </si>
+  <si>
+    <t>mariachi</t>
+  </si>
+  <si>
+    <t>jimboymartin</t>
+  </si>
+  <si>
+    <t>marine</t>
+  </si>
+  <si>
+    <t>smart</t>
+  </si>
+  <si>
+    <t>marites</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>marawi</t>
+  </si>
+  <si>
+    <t>marce</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>jumar</t>
+  </si>
+  <si>
+    <t>summarily</t>
+  </si>
+  <si>
+    <t>bbmarcos</t>
+  </si>
+  <si>
+    <t>marciano</t>
+  </si>
+  <si>
+    <t>mariing</t>
+  </si>
+  <si>
+    <t>mariah</t>
+  </si>
+  <si>
+    <t>tatamarin</t>
+  </si>
+  <si>
+    <t>mareplyan</t>
+  </si>
+  <si>
+    <t>marcosian</t>
+  </si>
+  <si>
+    <t>magmamartial</t>
+  </si>
+  <si>
+    <t>smarter</t>
+  </si>
+  <si>
+    <t>marcventures</t>
+  </si>
+  <si>
+    <t>marolio</t>
+  </si>
+  <si>
+    <t>mara</t>
+  </si>
+  <si>
+    <t>marino</t>
+  </si>
+  <si>
+    <t>marami</t>
+  </si>
+  <si>
+    <t>marielle</t>
+  </si>
+  <si>
+    <t>maraming</t>
+  </si>
+  <si>
+    <t>marunong</t>
+  </si>
+  <si>
+    <t>mararanasan</t>
+  </si>
+  <si>
+    <t>marasa</t>
+  </si>
+  <si>
+    <t>mare</t>
+  </si>
+  <si>
+    <t>maritime</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>maremember</t>
+  </si>
+  <si>
+    <t>maresolba</t>
+  </si>
+  <si>
+    <t>marcos​</t>
+  </si>
+  <si>
+    <t>maray</t>
+  </si>
+  <si>
+    <t>samar</t>
+  </si>
+  <si>
+    <t>bookmark</t>
+  </si>
+  <si>
+    <t>marayaw</t>
+  </si>
+  <si>
+    <t>submarine</t>
+  </si>
+  <si>
+    <t>marangal</t>
+  </si>
+  <si>
+    <t>namamaril</t>
+  </si>
+  <si>
+    <t>marco</t>
+  </si>
+  <si>
+    <t>remarkable</t>
+  </si>
+  <si>
+    <t>kaymariz</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>marka</t>
+  </si>
+  <si>
+    <t>market</t>
+  </si>
+  <si>
+    <t>bumaril</t>
+  </si>
+  <si>
+    <t>tamaraw</t>
+  </si>
+  <si>
+    <t>magmartial</t>
+  </si>
+  <si>
+    <t>maruhas</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>myanmar</t>
+  </si>
+  <si>
+    <t>marimar</t>
+  </si>
+  <si>
+    <t>margen</t>
+  </si>
+  <si>
+    <t>bongbongmarcos</t>
+  </si>
+  <si>
+    <t>march</t>
+  </si>
+  <si>
+    <t>smartmatic</t>
+  </si>
+  <si>
+    <t>maricaban</t>
+  </si>
+  <si>
+    <t>marinez</t>
+  </si>
+  <si>
+    <t>mariz</t>
+  </si>
+  <si>
+    <t>mariano</t>
+  </si>
+  <si>
+    <t>trademark</t>
+  </si>
+  <si>
+    <t>jejumar</t>
+  </si>
+  <si>
+    <t>jhonmarkgamon</t>
+  </si>
+  <si>
+    <t>maramin</t>
+  </si>
+  <si>
+    <t>roxases</t>
+  </si>
+  <si>
+    <t>mart</t>
+  </si>
+  <si>
+    <t>maricon</t>
+  </si>
+  <si>
+    <t>marijuana</t>
+  </si>
+  <si>
+    <t>camarines</t>
+  </si>
+  <si>
+    <t>maririnig</t>
+  </si>
+  <si>
+    <t>marcos</t>
+  </si>
+  <si>
+    <t>smartmagic</t>
+  </si>
+  <si>
+    <t>maramdaman</t>
+  </si>
+  <si>
+    <t>martinez</t>
+  </si>
+  <si>
+    <t>marginalized</t>
+  </si>
+  <si>
+    <t>kamara</t>
+  </si>
+  <si>
+    <t>marro</t>
+  </si>
+  <si>
+    <t>miriam</t>
+  </si>
+  <si>
+    <t>defensor</t>
+  </si>
   <si>
     <t>santiago</t>
-  </si>
-  <si>
-    <t>miriam</t>
-  </si>
-  <si>
-    <t>defensor</t>
   </si>
   <si>
     <t>©miriam</t>
@@ -377,6 +876,927 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A122"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -392,27 +1812,27 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>